<commit_message>
normalize survey response phone numbers
</commit_message>
<xml_diff>
--- a/scripts/numbers_example.xlsx
+++ b/scripts/numbers_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/code/nklugman/dumsorwatch/oink/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{5CAF4595-2465-ED43-81BB-061E7F543845}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{2AC29A38-98E8-2D4B-B72F-8AA9404A1BD3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{56ADAC23-6AC1-A34A-AA3D-CD22EBFE6C64}"/>
   </bookViews>
@@ -22,6 +22,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>+233558059073</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -55,8 +63,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -374,27 +383,31 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1">
+      <c r="A1" s="1">
         <v>558059583</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>552153084</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>558059073</v>
+      <c r="A3" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>